<commit_message>
Version 1.1. Change GUI and add some functions.
</commit_message>
<xml_diff>
--- a/ProbesCoeff.xlsx
+++ b/ProbesCoeff.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milenka\PycharmProjects\Keithley\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Milenka\PycharmProjects\Keithley - Skompilowane do exe\outputResTemp\TempMonitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84ED1578-CEA4-49B9-B411-8DCABD8A956E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3871BD3-3D45-404B-A389-D29F167E8A9A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7515" yWindow="795" windowWidth="14385" windowHeight="10740" xr2:uid="{D82E92BE-E042-4914-8041-82665EE820D3}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{D82E92BE-E042-4914-8041-82665EE820D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,6 +59,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
@@ -85,11 +93,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -404,19 +413,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB9B8714-B988-4A10-B4B8-75D36DC6489A}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="5" width="12.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -432,204 +442,185 @@
       <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" s="1"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>99.975999999999999</v>
+        <v>99.947705750748511</v>
       </c>
       <c r="C2">
-        <f>3.9083*10^-3</f>
-        <v>3.9083E-3</v>
+        <v>3.9068716813415259E-3</v>
       </c>
       <c r="D2">
-        <f>-5.775*10^-7</f>
-        <v>-5.7749999999999998E-7</v>
+        <v>-7.3330729419856932E-7</v>
       </c>
       <c r="E2">
         <f>-4.183*10^-12</f>
         <v>-4.1829999999999994E-12</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3">
-        <v>99.980999999999995</v>
+        <v>99.977521247312282</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:C11" si="0">3.9083*10^-3</f>
-        <v>3.9083E-3</v>
+        <v>3.9101785773457739E-3</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:D11" si="1">-5.775*10^-7</f>
-        <v>-5.7749999999999998E-7</v>
+        <v>-5.6922737128097572E-7</v>
       </c>
       <c r="E3">
-        <f t="shared" ref="E3:E11" si="2">-4.183*10^-12</f>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" ref="E3:E11" si="0">-4.183*10^-12</f>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4">
-        <v>99.974000000000004</v>
+        <v>99.965426321705834</v>
       </c>
       <c r="C4">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.9122545080345879E-3</v>
       </c>
       <c r="D4">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-6.1500446041687692E-7</v>
       </c>
       <c r="E4">
-        <f t="shared" si="2"/>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>99.981999999999999</v>
+        <v>99.964147566469393</v>
       </c>
       <c r="C5">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.9081300894337184E-3</v>
       </c>
       <c r="D5">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-6.1712370636251645E-7</v>
       </c>
       <c r="E5">
-        <f t="shared" si="2"/>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6">
-        <v>100.003</v>
+        <v>99.997828425063204</v>
       </c>
       <c r="C6">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.911830491871637E-3</v>
       </c>
       <c r="D6">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-5.9808748728980255E-7</v>
       </c>
       <c r="E6">
-        <f t="shared" si="2"/>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7">
-        <v>99.998999999999995</v>
+        <v>99.994271188017294</v>
       </c>
       <c r="C7">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.9112043883100557E-3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-5.8740243205481353E-7</v>
       </c>
       <c r="E7">
-        <f t="shared" si="2"/>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8">
-        <v>99.989000000000004</v>
+        <v>99.982094052063857</v>
       </c>
       <c r="C8">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.9115431734577039E-3</v>
       </c>
       <c r="D8">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-5.9134767555764435E-7</v>
       </c>
       <c r="E8">
-        <f t="shared" si="2"/>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9">
-        <v>100.001</v>
+        <v>99.995996343648926</v>
       </c>
       <c r="C9">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.9108376097579311E-3</v>
       </c>
       <c r="D9">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-5.7461163465562884E-7</v>
       </c>
       <c r="E9">
-        <f t="shared" si="2"/>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10">
-        <v>100.002</v>
+      <c r="B10" s="2">
+        <v>100.005008807946</v>
       </c>
       <c r="C10">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.9090684189565768E-3</v>
       </c>
       <c r="D10">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-6.7100790690791566E-7</v>
       </c>
       <c r="E10">
-        <f t="shared" si="2"/>
-        <v>-4.1829999999999994E-12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>-4.1829999999999994E-12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11">
-        <v>100</v>
+        <v>99.979722735358422</v>
       </c>
       <c r="C11">
-        <f t="shared" si="0"/>
-        <v>3.9083E-3</v>
+        <v>3.9114640360913651E-3</v>
       </c>
       <c r="D11">
-        <f t="shared" si="1"/>
-        <v>-5.7749999999999998E-7</v>
+        <v>-5.8245200330939762E-7</v>
       </c>
       <c r="E11">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>-4.1829999999999994E-12</v>
       </c>
     </row>

</xml_diff>